<commit_message>
Gantt chart excel spreadsheet.
</commit_message>
<xml_diff>
--- a/gantt_chart.xlsx
+++ b/gantt_chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Klodi\Documents\computer-science-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{76F03B4A-FB12-4C1B-A8E3-0A2DEA2CB172}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7612CFF2-E7BF-4657-B4BD-41B8B6C7898B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{C58E1C32-9496-4ECA-BE91-6E09D7F0AB41}"/>
   </bookViews>
@@ -1463,14 +1463,14 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
     <col min="2" max="3" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
     <col min="7" max="7" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>